<commit_message>
fix logic price & replace tempat wisata
</commit_message>
<xml_diff>
--- a/public/template/template-wisata.xlsx
+++ b/public/template/template-wisata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wisata_bwx\public\asset\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wisata_bwx\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC6D8257-5AF4-4527-90A4-4CCA3FAB0E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2760229E-BCC9-492F-A069-F0220857C9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{ACEB36B4-5654-4331-9719-A1F77C787DA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>nama_tempat_wisata</t>
   </si>
@@ -60,9 +60,6 @@
     <t>pantai indah</t>
   </si>
   <si>
-    <t>1,2,6,3,4,7</t>
-  </si>
-  <si>
     <t>Kawah Ijen</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Gunung Indah</t>
   </si>
   <si>
-    <t>1,2,3,4,5</t>
-  </si>
-  <si>
     <t>Banyuwangi Park</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Wisata Alam Sabana</t>
   </si>
   <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
     <t>Taman Nasional Alas Purwo</t>
   </si>
   <si>
@@ -108,7 +99,13 @@
     <t>Wisata Alam Asri</t>
   </si>
   <si>
-    <t>1,2,3,4,6,7</t>
+    <t>9,7,2,1,4</t>
+  </si>
+  <si>
+    <t>9,7,6,2,1,3,4</t>
+  </si>
+  <si>
+    <t>9,7,2,1</t>
   </si>
 </sst>
 </file>
@@ -177,6 +174,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19878D20-C308-962A-0223-CFF210F6ABE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7315200" y="1289050"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,7 +529,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,13 +562,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2">
         <v>4.7</v>
@@ -530,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -553,18 +603,18 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>4.5</v>
@@ -576,18 +626,18 @@
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5">
         <v>4.5999999999999996</v>
@@ -599,18 +649,18 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>4.5999999999999996</v>
@@ -622,11 +672,12 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>